<commit_message>
Updated databases so they are matching (From now edit only using console commands)
</commit_message>
<xml_diff>
--- a/src/database/BookingHistory.xlsx
+++ b/src/database/BookingHistory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohsh\Documents\GitHub\SC2002_Assignment\src\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A429D4B0-7D56-47D5-972D-9AFABD10B3C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F7C4D63-1947-4744-AD79-52E1B9588DCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{83934A19-CB5D-49C7-89C5-6A46A7FDD360}"/>
   </bookViews>
@@ -62,13 +62,13 @@
     <t/>
   </si>
   <si>
-    <t>shing</t>
+    <t>shinghao</t>
   </si>
   <si>
     <t>91234567</t>
   </si>
   <si>
-    <t>shing@gmail.com</t>
+    <t>sohshinghao@gmail.com</t>
   </si>
   <si>
     <t>D01</t>
@@ -430,7 +430,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,10 +498,10 @@
         <v>12</v>
       </c>
       <c r="F3" t="n" s="0">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G3" t="n" s="0">
-        <v>10.0</v>
+        <v>26.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Re-organise files to Model-View-Controller
</commit_message>
<xml_diff>
--- a/src/database/BookingHistory.xlsx
+++ b/src/database/BookingHistory.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="13">
   <si>
     <t>Username</t>
   </si>
@@ -427,7 +427,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E77177D7-C16B-48D5-B7B1-B9ED6489238F}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
@@ -527,6 +527,29 @@
         <v>96.0</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="F5" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="G5" t="n" s="0">
+        <v>48.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>